<commit_message>
carcase javascript images processor
</commit_message>
<xml_diff>
--- a/docs/backlog (Автосохраненный).xlsx
+++ b/docs/backlog (Автосохраненный).xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Чистильчик мусора, для файлов не удаленных во время, смотреть дату файла</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>Подключить систему шаблонов для js</t>
+  </si>
+  <si>
+    <t>Офлайн режим работы</t>
   </si>
 </sst>
 </file>
@@ -400,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,6 +469,11 @@
         <v>10</v>
       </c>
     </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>